<commit_message>
commiting for data selecting
</commit_message>
<xml_diff>
--- a/OS_test_sorter.xlsx
+++ b/OS_test_sorter.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25122"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E282F182-0E09-439D-B37F-218E37EF41F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA0EEDB4-7B47-44F4-BE02-4D48F05463DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>OS1</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>OS4</t>
+  </si>
+  <si>
+    <t>OS5</t>
+  </si>
+  <si>
+    <t>OS6</t>
+  </si>
+  <si>
+    <t>OS7</t>
   </si>
 </sst>
 </file>
@@ -402,159 +411,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C24"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:C24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="B3" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" t="s">
+      <c r="B2">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" t="s">
+      <c r="B3">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" t="s">
+      <c r="B4">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" t="s">
+      <c r="B5">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
-      <c r="B9" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="C9">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="B10" t="s">
+      <c r="B8">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="C10">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" t="s">
+      <c r="B9">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="C11">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" t="s">
+      <c r="B10">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="C12">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="B14" t="s">
+      <c r="B11">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
-      <c r="B15" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="C15">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3">
-      <c r="B16" t="s">
+      <c r="B14">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="C16">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" t="s">
+      <c r="B15">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="C17">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" t="s">
+      <c r="B16">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="C18">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" t="s">
+      <c r="B17">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
-      <c r="B21" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="C21">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" t="s">
+      <c r="B20">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="C22">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" t="s">
+      <c r="B21">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>3</v>
       </c>
-      <c r="C23">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" t="s">
+      <c r="B22">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="C24">
+      <c r="B23">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41">
         <v>0.23400000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commiting for selecting data. incomplete version!
</commit_message>
<xml_diff>
--- a/OS_test_sorter.xlsx
+++ b/OS_test_sorter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25122"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA0EEDB4-7B47-44F4-BE02-4D48F05463DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C1D6B5D-2D21-444D-87FD-1BF0E046D8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="11">
   <si>
     <t>OS1</t>
   </si>
@@ -411,268 +411,438 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:D41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="B15">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="B16">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>1</v>
       </c>
       <c r="B20">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>2</v>
       </c>
       <c r="B21">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>3</v>
       </c>
       <c r="B22">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>1</v>
       </c>
       <c r="B26">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>2</v>
       </c>
       <c r="B27">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>4</v>
       </c>
       <c r="B29">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>1</v>
       </c>
       <c r="B32">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>2</v>
       </c>
       <c r="B33">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>3</v>
       </c>
       <c r="B34">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>4</v>
       </c>
       <c r="B35">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>1</v>
       </c>
       <c r="B38">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>2</v>
       </c>
       <c r="B39">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>3</v>
       </c>
       <c r="B40">
         <v>0.23400000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>4</v>
       </c>
       <c r="B41">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41">
         <v>0.23400000000000001</v>
       </c>
     </row>

</xml_diff>